<commit_message>
added esp to BOM
</commit_message>
<xml_diff>
--- a/Rev 3/BOM.xlsx
+++ b/Rev 3/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5d13c61c60eae0c/Documents/College/IEEE/MP3 Player/2024-IEEE-MP3-Project/Rev 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{FDAF1807-9717-4964-B21E-4ECFEDE555D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A0090B9-FFF5-4D6F-90C4-20FA909359B2}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{FDAF1807-9717-4964-B21E-4ECFEDE555D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DB49977-B82D-4BD8-B722-999521A84E15}"/>
   <bookViews>
     <workbookView xWindow="5268" yWindow="2076" windowWidth="17280" windowHeight="9960" xr2:uid="{690C5F81-271B-4348-BD0D-3A1EC7B2575C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Comment</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>C26985</t>
+  </si>
+  <si>
+    <t>ESP 32 S3 Wroom N16R8</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1-N16R8</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>C2913202</t>
   </si>
 </sst>
 </file>
@@ -598,15 +610,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE193435-DF19-4D96-AD24-044B4D184BAE}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
@@ -724,7 +736,22 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>